<commit_message>
Add blog management scripts and new blog post
- Add blog:add and blog:sync npm scripts for managing posts via Excel
- Add xlsx dependency for Excel parsing
- Add update-blog script for adding/syncing blog posts
- Add new blog post: "Everyone should be using Claude Code more"
- Update CLAUDE.md with blog post workflow documentation

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/Blog.xlsx
+++ b/src/Blog.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29712"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29713"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIRECTORY\Claude Code\claude-code-playbooks\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99090C6-D194-4F3B-B17F-235020234512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918B4BF1-BF06-4672-BF91-5D80FB52EEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blog Posts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>title</t>
   </si>
@@ -79,35 +74,48 @@
   </si>
   <si>
     <t>plan mode; assistant; workflow; commands</t>
+  </si>
+  <si>
+    <t>Everyone should be using Claude Code more</t>
+  </si>
+  <si>
+    <t>A practical guide exploring Claude Code as an underutilized AI tool for non-technical users, with installation instructions and 50 real-world applications ranging from file organization to business automation.</t>
+  </si>
+  <si>
+    <t>guide</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>https://www.lennysnewsletter.com/p/everyone-should-be-using-claude-code</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>getting started</t>
+  </si>
+  <si>
+    <t>claude code; productivity; automation; non-technical; file management; business</t>
+  </si>
+  <si>
+    <t>2026-01-29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -128,29 +136,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -173,44 +170,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -240,12 +237,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -284,207 +281,266 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="51.21875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="60.796875" customWidth="1"/>
+    <col min="2" max="2" width="80.796875" customWidth="1"/>
+    <col min="3" max="3" width="12.796875" customWidth="1"/>
+    <col min="4" max="5" width="14.796875" customWidth="1"/>
+    <col min="6" max="6" width="80.796875" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" customWidth="1"/>
+    <col min="8" max="8" width="12.796875" customWidth="1"/>
+    <col min="9" max="9" width="20.796875" customWidth="1"/>
+    <col min="10" max="10" width="40.796875" customWidth="1"/>
+    <col min="11" max="11" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -496,7 +552,7 @@
       <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2" t="b">
@@ -508,17 +564,52 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="1">
         <v>46043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{E9AB00A3-7892-4010-8498-9379AFD274E9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:K3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Nate's "Wait, I Can Use Claude Code" guide to blog posts
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/Blog.xlsx
+++ b/src/Blog.xlsx
@@ -1,116 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIRECTORY\Claude Code\claude-code-playbooks\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918B4BF1-BF06-4672-BF91-5D80FB52EEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Blog Posts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>difficulty</t>
-  </si>
-  <si>
-    <t>readingTime</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>featured</t>
-  </si>
-  <si>
-    <t>thumbnailType</t>
-  </si>
-  <si>
-    <t>thumbnailTitle</t>
-  </si>
-  <si>
-    <t>tags</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>How to Turn Claude Code Into Your Personal AI Assistant</t>
-  </si>
-  <si>
-    <t>Tutorial on how you can transform Claude from a chatbot into a powerful personal chief of staff that lives on your computer—organizing files, conducting deep research, and managing your knowledge base autonomously.</t>
-  </si>
-  <si>
-    <t>agent</t>
-  </si>
-  <si>
-    <t>intermediate</t>
-  </si>
-  <si>
-    <t>https://www.theneuron.ai/explainer-articles/how-to-turn-claude-code-into-your-personal-ai-assistant</t>
-  </si>
-  <si>
-    <t>work assistant</t>
-  </si>
-  <si>
-    <t>plan mode; assistant; workflow; commands</t>
-  </si>
-  <si>
-    <t>Everyone should be using Claude Code more</t>
-  </si>
-  <si>
-    <t>A practical guide exploring Claude Code as an underutilized AI tool for non-technical users, with installation instructions and 50 real-world applications ranging from file organization to business automation.</t>
-  </si>
-  <si>
-    <t>guide</t>
-  </si>
-  <si>
-    <t>basic</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>https://www.lennysnewsletter.com/p/everyone-should-be-using-claude-code</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>getting started</t>
-  </si>
-  <si>
-    <t>claude code; productivity; automation; non-technical; file management; business</t>
-  </si>
-  <si>
-    <t>2026-01-29</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,23 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -480,136 +396,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.796875" customWidth="1"/>
-    <col min="2" max="2" width="80.796875" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" customWidth="1"/>
-    <col min="4" max="5" width="14.796875" customWidth="1"/>
-    <col min="6" max="6" width="80.796875" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
-    <col min="9" max="9" width="20.796875" customWidth="1"/>
-    <col min="10" max="10" width="40.796875" customWidth="1"/>
-    <col min="11" max="11" width="12.796875" customWidth="1"/>
+    <col min="1" max="1" width="60.83203125" customWidth="1"/>
+    <col min="2" max="2" width="80.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="80.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="40.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>title</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>category</v>
+      </c>
+      <c r="D1" t="str">
+        <v>difficulty</v>
+      </c>
+      <c r="E1" t="str">
+        <v>readingTime</v>
+      </c>
+      <c r="F1" t="str">
+        <v>url</v>
+      </c>
+      <c r="G1" t="str">
+        <v>featured</v>
+      </c>
+      <c r="H1" t="str">
+        <v>thumbnailType</v>
+      </c>
+      <c r="I1" t="str">
+        <v>thumbnailTitle</v>
+      </c>
+      <c r="J1" t="str">
+        <v>tags</v>
+      </c>
+      <c r="K1" t="str">
+        <v>createdAt</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>How to Turn Claude Code Into Your Personal AI Assistant</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Tutorial on how you can transform Claude from a chatbot into a powerful personal chief of staff that lives on your computer—organizing files, conducting deep research, and managing your knowledge base autonomously.</v>
+      </c>
+      <c r="C2" t="str">
+        <v>agent</v>
+      </c>
+      <c r="D2" t="str">
+        <v>intermediate</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
+      <c r="F2" t="str">
+        <v>https://www.theneuron.ai/explainer-articles/how-to-turn-claude-code-into-your-personal-ai-assistant</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="H2" t="str">
+        <v>agent</v>
+      </c>
+      <c r="I2" t="str">
+        <v>work assistant</v>
+      </c>
+      <c r="J2" t="str">
+        <v>plan mode; assistant; workflow; commands</v>
+      </c>
+      <c r="K2">
         <v>46043</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Everyone should be using Claude Code more</v>
+      </c>
+      <c r="B3" t="str">
+        <v>A practical guide exploring Claude Code as an underutilized AI tool for non-technical users, with installation instructions and 50 real-world applications ranging from file organization to business automation.</v>
+      </c>
+      <c r="C3" t="str">
+        <v>guide</v>
+      </c>
+      <c r="D3" t="str">
+        <v>basic</v>
+      </c>
+      <c r="E3" t="str">
+        <v>12</v>
+      </c>
+      <c r="F3" t="str">
+        <v>https://www.lennysnewsletter.com/p/everyone-should-be-using-claude-code</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
+      <c r="H3" t="str">
+        <v>default</v>
+      </c>
+      <c r="I3" t="str">
+        <v>getting started</v>
+      </c>
+      <c r="J3" t="str">
+        <v>claude code; productivity; automation; non-technical; file management; business</v>
+      </c>
+      <c r="K3" t="str">
+        <v>2026-01-29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>The Complete Wait, I Can Use Claude Code Guide</v>
+      </c>
+      <c r="B4" t="str">
+        <v>A comprehensive guide arguing that Claude Code is a productivity tool for non-developers, featuring browser automation, Slack integration, and workflow capabilities with practical frameworks for iterative AI collaboration.</v>
+      </c>
+      <c r="C4" t="str">
+        <v>guide</v>
+      </c>
+      <c r="D4" t="str">
+        <v>basic</v>
+      </c>
+      <c r="E4" t="str">
+        <v>15 min read</v>
+      </c>
+      <c r="F4" t="str">
+        <v>https://natesnewsletter.substack.com/p/the-complete-wait-i-can-use-claude</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>default</v>
+      </c>
+      <c r="I4" t="str">
+        <v>getting started</v>
+      </c>
+      <c r="J4" t="str">
+        <v>claude code;productivity;non-technical;automation;browser automation;workflow</v>
+      </c>
+      <c r="K4" t="str">
+        <v>2025-12-22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K3" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Product Talk blog post about Claude Code
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/Blog.xlsx
+++ b/src/Blog.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -555,9 +555,44 @@
         <v>2025-12-22</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Claude Code: What It Is and How It's Different</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Teresa Torres explains Claude Code as a terminal-based AI tool that differs from browser-based Claude, highlighting benefits like automatic file access, local data storage, reusable slash commands, and parallel agent processing.</v>
+      </c>
+      <c r="C5" t="str">
+        <v>guide</v>
+      </c>
+      <c r="D5" t="str">
+        <v>basic</v>
+      </c>
+      <c r="E5" t="str">
+        <v>8</v>
+      </c>
+      <c r="F5" t="str">
+        <v>https://www.producttalk.org/claude-code-what-it-is-and-how-its-different/</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>default</v>
+      </c>
+      <c r="I5" t="str">
+        <v>What is Claude Code</v>
+      </c>
+      <c r="J5" t="str">
+        <v>claude code; terminal; getting started; non-technical; file access; agents</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-03</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Armin Ronacher's Agentic Coding Recommendations blog post
Co-Authored-By: Claude (claude-opus-4-6) <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/Blog.xlsx
+++ b/src/Blog.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -590,9 +590,79 @@
         <v>2026-02-03</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>How I Use Every Claude Code Feature</v>
+      </c>
+      <c r="B6" t="str">
+        <v>A comprehensive practitioner's guide to every Claude Code feature, from CLAUDE.md configuration to hooks, planning mode, skills, MCP, and enterprise GitHub Actions workflows.</v>
+      </c>
+      <c r="C6" t="str">
+        <v>guide</v>
+      </c>
+      <c r="D6" t="str">
+        <v>advanced</v>
+      </c>
+      <c r="E6" t="str">
+        <v>15</v>
+      </c>
+      <c r="F6" t="str">
+        <v>https://blog.sshh.io/p/how-i-use-every-claude-code-feature</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <v>skill</v>
+      </c>
+      <c r="I6" t="str">
+        <v>All Features</v>
+      </c>
+      <c r="J6" t="str">
+        <v>CLAUDE.md; hooks; planning mode; skills; MCP; custom commands; subagents; GitHub Actions; SDK; enterprise</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-02-06</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Agentic Coding Recommendations — Armin Ronacher</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Flask creator Armin Ronacher shares practical recommendations for agentic coding, covering language choices, tool design, observability, and code organization for AI-driven development.</v>
+      </c>
+      <c r="C7" t="str">
+        <v>guide</v>
+      </c>
+      <c r="D7" t="str">
+        <v>intermediate</v>
+      </c>
+      <c r="E7" t="str">
+        <v>12</v>
+      </c>
+      <c r="F7" t="str">
+        <v>https://lucumr.pocoo.org/2025/6/12/agentic-coding/</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>agent</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Agentic Coding</v>
+      </c>
+      <c r="J7" t="str">
+        <v>agentic coding; Go; Python; tooling; observability; refactoring; workflow</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-07</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>